<commit_message>
Melhorias de vida substâncias
Implementação de busca dos valores das colunas por índice;

Validação de emails a serem enviados antes dos envios começarem;

Melhorias de lógica, nomes de variáveis e parâmetros
</commit_message>
<xml_diff>
--- a/Disparador com Anexo/src/static/Enviar E-mails.xlsx
+++ b/Disparador com Anexo/src/static/Enviar E-mails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Códigos\Projeto-Envio-Email\Disparador com Anexo\src\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabela.borges\Desktop\Disparador com anexo\src\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D084EB91-35C0-4B8E-BF89-B400D8881D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25F5D9E-010C-4AB0-A349-0499493622BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>E-mail</t>
   </si>
@@ -34,10 +34,22 @@
     <t>Protocolo</t>
   </si>
   <si>
+    <t>Nome_arquivos_anexo</t>
+  </si>
+  <si>
     <t>STATUS</t>
   </si>
   <si>
-    <t>PDF</t>
+    <t>oversouls11@gmail.com</t>
+  </si>
+  <si>
+    <t>financeiro4@webcertificados.com.br</t>
+  </si>
+  <si>
+    <t>308828.pdf</t>
+  </si>
+  <si>
+    <t>123456.pdf;21372.pdf</t>
   </si>
 </sst>
 </file>
@@ -400,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,10 +441,26 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>